<commit_message>
Some finishing touches to the board
</commit_message>
<xml_diff>
--- a/Electrical/MainBoard/bom/bom_additional_digikey_components.xlsx
+++ b/Electrical/MainBoard/bom/bom_additional_digikey_components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satom\Desktop\Robot\Electrical\MainBoard\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCB36DE-2A77-4B7C-978A-64F9A2437401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AB5FFB-6841-4AB2-B6E8-D5C136529140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="12318" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>WM2002-ND</t>
+  </si>
+  <si>
+    <t>WM4622-ND</t>
+  </si>
+  <si>
+    <t>Main Power Male</t>
+  </si>
+  <si>
+    <t>Main Power Female</t>
+  </si>
+  <si>
+    <t>Main Power Crimp</t>
+  </si>
+  <si>
+    <t>WM2124-ND</t>
+  </si>
+  <si>
+    <t>WM20948CT-ND</t>
   </si>
 </sst>
 </file>
@@ -153,9 +171,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -503,7 +520,7 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3">
@@ -719,6 +736,66 @@
       </c>
       <c r="F14">
         <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>26604040</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>9508041</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>8500008</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>